<commit_message>
arreglos en mapeo fisico y estructura del diagrama E/R
</commit_message>
<xml_diff>
--- a/Diagrama de tablas IPC2 Proyecto 1 .xlsx
+++ b/Diagrama de tablas IPC2 Proyecto 1 .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA89BE38-63CA-486E-8353-1B074DBC53BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEEAFD1-1A67-4D59-B2EA-E31127531AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7140" yWindow="495" windowWidth="10920" windowHeight="7785" xr2:uid="{AC607708-AF35-4EB0-AAB4-58680187AFD8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AC607708-AF35-4EB0-AAB4-58680187AFD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="67">
   <si>
     <t>Entidad Usuario</t>
   </si>
@@ -216,6 +216,27 @@
   </si>
   <si>
     <t>id_usuario</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>Entidad Taller</t>
+  </si>
+  <si>
+    <t>PRIMARIA/FORANEA</t>
+  </si>
+  <si>
+    <t>cupo_maximo</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>cupo_disponible</t>
+  </si>
+  <si>
+    <t>cupo_reservado</t>
   </si>
 </sst>
 </file>
@@ -625,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4AED79-0445-47AE-AABD-19737B42F24D}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:I19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +658,7 @@
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="38.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -880,10 +902,10 @@
       <c r="G15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="4" t="s">
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -906,10 +928,10 @@
       <c r="G16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="4" t="s">
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -932,10 +954,10 @@
       <c r="G17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="4" t="s">
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -958,10 +980,10 @@
       <c r="G18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="4" t="s">
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -984,10 +1006,10 @@
       <c r="G19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="4" t="s">
+      <c r="H19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1047,6 +1069,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>43</v>
@@ -1100,16 +1136,16 @@
       <c r="E28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="4" t="s">
+      <c r="I28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1117,7 +1153,7 @@
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1129,30 +1165,30 @@
       <c r="E29" s="2">
         <v>35</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J29" s="4" t="s">
+      <c r="I29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="4" t="s">
+      <c r="I30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1346,6 +1382,9 @@
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="F46" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -1360,6 +1399,18 @@
       <c r="D47" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
@@ -1374,8 +1425,20 @@
       <c r="D48" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F48" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -1387,6 +1450,32 @@
       </c>
       <c r="D49" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcion de diagrama E/R
</commit_message>
<xml_diff>
--- a/Diagrama de tablas IPC2 Proyecto 1 .xlsx
+++ b/Diagrama de tablas IPC2 Proyecto 1 .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Documents\Proyecto_1_IPC2_JulioOvalle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEEAFD1-1A67-4D59-B2EA-E31127531AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD90D1A-9F5A-426B-9101-691252F13AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AC607708-AF35-4EB0-AAB4-58680187AFD8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="67">
   <si>
     <t>Entidad Usuario</t>
   </si>
@@ -218,9 +218,6 @@
     <t>id_usuario</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>Entidad Taller</t>
   </si>
   <si>
@@ -236,7 +233,10 @@
     <t>cupo_disponible</t>
   </si>
   <si>
-    <t>cupo_reservado</t>
+    <t>contraseña</t>
+  </si>
+  <si>
+    <t>Entidad Reserva</t>
   </si>
 </sst>
 </file>
@@ -306,12 +306,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4AED79-0445-47AE-AABD-19737B42F24D}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,6 +663,7 @@
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="38.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -735,7 +741,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>24</v>
@@ -806,6 +812,9 @@
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -820,6 +829,18 @@
       <c r="D8" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -834,6 +855,18 @@
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -848,6 +881,44 @@
       <c r="D10" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1070,18 +1141,10 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -1162,7 +1225,7 @@
       <c r="D29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="5">
         <v>35</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -1179,6 +1242,21 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="G30" s="2" t="s">
         <v>48</v>
       </c>
@@ -1190,6 +1268,20 @@
       </c>
       <c r="J30" s="2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1234,7 +1326,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>24</v>
@@ -1260,7 +1352,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>24</v>
@@ -1296,21 +1388,24 @@
       <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
       <c r="F40" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F41" s="1" t="s">
@@ -1327,16 +1422,16 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="B42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F42" s="2" t="s">
@@ -1353,16 +1448,16 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="C43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F43" s="2" t="s">
@@ -1383,7 +1478,7 @@
         <v>56</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -1435,7 +1530,7 @@
         <v>17</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -1452,10 +1547,10 @@
         <v>24</v>
       </c>
       <c r="F49" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>17</v>
@@ -1466,10 +1561,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F50" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
creacion de login y avances con vista del admin del sistema
</commit_message>
<xml_diff>
--- a/Diagrama de tablas IPC2 Proyecto 1 .xlsx
+++ b/Diagrama de tablas IPC2 Proyecto 1 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Documents\Proyecto_1_IPC2_JulioOvalle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07A5288-9B25-4C93-8EA8-6904B26E19B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1158DDD5-811E-4B4D-8646-CA4939F3B0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AC607708-AF35-4EB0-AAB4-58680187AFD8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="73">
   <si>
     <t>Entidad Usuario</t>
   </si>
@@ -237,6 +237,24 @@
   </si>
   <si>
     <t>Entidad Reserva</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>Entidad Configuracion_ganancia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INT </t>
+  </si>
+  <si>
+    <t>total_recaudado</t>
+  </si>
+  <si>
+    <t>total_ganancia</t>
+  </si>
+  <si>
+    <t>porcentaje_comision</t>
   </si>
 </sst>
 </file>
@@ -306,17 +324,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,15 +667,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4AED79-0445-47AE-AABD-19737B42F24D}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="97" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="38.5703125" customWidth="1"/>
@@ -895,19 +911,19 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1140,12 +1156,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>43</v>
@@ -1217,7 +1227,7 @@
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>17</v>
@@ -1225,7 +1235,7 @@
       <c r="D29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <v>35</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -1242,19 +1252,19 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="B30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -1271,16 +1281,16 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" s="4" t="s">
+      <c r="H31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1384,192 +1394,270 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="F40" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D43" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="4" t="s">
+      <c r="B44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="H44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="G45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="C50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I48" s="2" t="s">
+      <c r="H50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="2" t="s">
+      <c r="B51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F50" s="2" t="s">
+      <c r="H51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F52" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I50" s="2" t="s">
+      <c r="H52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>